<commit_message>
round 1: Glob vs. lok
</commit_message>
<xml_diff>
--- a/LL.xlsx
+++ b/LL.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>.</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>$</t>
+  </si>
+  <si>
+    <t>GLOBDEKDAL</t>
+  </si>
+  <si>
+    <t>GLOBDEK</t>
   </si>
 </sst>
 </file>
@@ -483,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A9:Z29"/>
+  <dimension ref="A9:Z31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -606,7 +612,7 @@
     </row>
     <row r="11" spans="1:26">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C11">
         <v>29</v>
@@ -844,7 +850,7 @@
     </row>
     <row r="28" spans="1:25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C28">
         <v>30</v>
@@ -865,6 +871,28 @@
       </c>
       <c r="Y29">
         <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q30">
+        <v>40</v>
+      </c>
+      <c r="T30">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31">
+        <v>42</v>
+      </c>
+      <c r="Q31">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>